<commit_message>
Updated hour log and added introduciton files
</commit_message>
<xml_diff>
--- a/Uren log.xlsx
+++ b/Uren log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\shipping-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B47B3D-B0D7-4B2A-A085-FE12EAE2AAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E1BFBD-36F6-4B74-81BC-AE7D36915E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ewout" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Wanneer</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Study</t>
+  </si>
+  <si>
+    <t>Searching data</t>
   </si>
 </sst>
 </file>
@@ -433,14 +436,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC13614-0EFB-42A2-B55B-3B7A8DE84ACE}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -477,6 +481,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44832</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Maersk fill in form (ie RTM Santos)
</commit_message>
<xml_diff>
--- a/Uren log.xlsx
+++ b/Uren log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Documents\Github\shipping-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C24B813-F8F0-4BD7-B085-4F264817221B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62022F1C-2A40-4386-BF70-93D96D9A5B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{04463C6E-4673-4318-950F-02DFA8CEE6E5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>Wanneer</t>
   </si>
@@ -63,7 +63,7 @@
     <t>Datascraper</t>
   </si>
   <si>
-    <t>3.5</t>
+    <t>1.5</t>
   </si>
 </sst>
 </file>
@@ -442,9 +442,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC13614-0EFB-42A2-B55B-3B7A8DE84ACE}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -485,8 +487,8 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <f>SUM(C2:C10)</f>
-        <v>8</v>
+        <f>SUM(C2:C15)</f>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -556,8 +558,47 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44845</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44846</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44853</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44853</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>